<commit_message>
Update the behavior of OutputExcel function in vue tables in order to make it more multilingual friendly. OutboundBackrecordTable & OutboundPickrecordTable WIP InboundSearchTable WIP
</commit_message>
<xml_diff>
--- a/public/download/MaterialExample.xlsx
+++ b/public/download/MaterialExample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>料號</t>
   </si>
@@ -70,7 +70,10 @@
     <t>pcs</t>
   </si>
   <si>
-    <t>是</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t>IE備品室</t>
@@ -91,7 +94,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -123,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -138,10 +141,13 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,10 +469,10 @@
     <col min="10" max="10" style="5" width="15.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="5" width="15.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="5" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21.75">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -539,10 +545,10 @@
         <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="4"/>
     </row>

</xml_diff>